<commit_message>
add case op but no check and compile
</commit_message>
<xml_diff>
--- a/datapath/信号表.xlsx
+++ b/datapath/信号表.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="286">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -452,23 +452,247 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>JR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JRRA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RPC(PC+1?)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100</t>
+    <t>RA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sign(inst(4 downto 0))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mem_addr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LW_SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mem[mem_addr]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mem[mem_addr]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MFIH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[x]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MFPC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_read</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg2_read</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTIH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTSP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -476,11 +700,371 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>JRRA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010010</t>
+    <t>reg1_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~reg1_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[y]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data | reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data + reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data + reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data + reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data &amp; reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data = 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data != 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data = 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data != 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data != reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data != reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data + reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data - reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLLV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[y]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data &lt;&lt; reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[y]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data &lt;&lt; reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[x]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data &lt; reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLTI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data &lt; reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有符号比较</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLTU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[y]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data &lt; reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLTUI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无符号比较</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sign(inst(4 downto 2))(0=&gt;8)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data &gt;&gt; reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRAV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算术右移</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRLV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sign(inst(4 downto 2))(0=&gt;8)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data &gt;&gt; reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逻辑右移</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[y]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data &gt;&gt; reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUBU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data - reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW_RS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mem_write_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -488,15 +1072,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>sign(inst(4 downto 0))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>RA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010011</t>
+    <t>SW_SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sign(inst(7 downto 0))</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -504,23 +1104,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sign(inst(4 downto 0))</t>
+    <t>reg1_data+reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data ^ reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDSP3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zero(inst(7 downto 0))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">条件满足时要把延迟槽里的指令清空（具体实现：控制信号置0？）                                                 条件不满足时banch_flag=0 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -528,643 +1156,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>mem_addr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LW_SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mem[mem_addr]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mem[mem_addr]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MFIH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R[x]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MFPC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MOVE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_read</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg2_read</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MTIH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MTSP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NEG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NOT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>~reg1_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NOP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R[y]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data | reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data + reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data + reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data + reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data &amp; reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data = 0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data != 0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data = 0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data != 0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data != reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data != reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data + reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data - reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLLV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R[y]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data &lt;&lt; reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R[y]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data &lt;&lt; reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R[x]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data &lt; reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLTI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data &lt; reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有符号比较</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLTU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R[y]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data &lt; reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLTUI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无符号比较</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SRA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sign(inst(4 downto 2))(0=&gt;8)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data &gt;&gt; reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SRAV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>算术右移</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SRL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SRLV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sign(inst(4 downto 2))(0=&gt;8)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data &gt;&gt; reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>逻辑右移</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R[y]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data &gt;&gt; reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SUBU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>z</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data - reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SW_RS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mem_write_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sign(inst(4 downto 0))</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SW_SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sign(inst(7 downto 0))</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data+reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XOR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>z</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data ^ reg2_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADDSP3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>zero(inst(7 downto 0))</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1_data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">条件满足时要把延迟槽里的指令清空（具体实现：控制信号置0？）                                                 条件不满足时banch_flag=0 </t>
+    <t>PC+2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg2_data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC+1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1513,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9:Q12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1549,7 +1557,7 @@
         <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>64</v>
@@ -1558,7 +1566,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>65</v>
@@ -1576,10 +1584,10 @@
         <v>15</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>1</v>
@@ -1621,7 +1629,7 @@
         <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1663,7 +1671,7 @@
         <v>34</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1674,7 +1682,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>35</v>
@@ -1705,7 +1713,7 @@
         <v>39</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1747,7 +1755,7 @@
         <v>85</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1791,7 +1799,7 @@
         <v>45</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1811,7 +1819,7 @@
         <v>52</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>29</v>
@@ -1835,7 +1843,7 @@
         <v>14</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1900,7 +1908,7 @@
         <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
@@ -1911,7 +1919,7 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1922,7 +1930,7 @@
         <v>28</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1956,7 +1964,7 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1988,7 +1996,7 @@
         <v>75</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
@@ -1999,7 +2007,7 @@
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -2022,7 +2030,7 @@
         <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>79</v>
@@ -2042,7 +2050,7 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -2087,7 +2095,7 @@
         <v>74</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2107,7 +2115,7 @@
         <v>89</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>14</v>
@@ -2129,7 +2137,7 @@
         <v>90</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2185,15 +2193,17 @@
         <v>18</v>
       </c>
       <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="J16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>105</v>
+        <v>281</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>106</v>
+        <v>283</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -2206,13 +2216,13 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>28</v>
@@ -2236,7 +2246,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>81</v>
@@ -2244,22 +2254,22 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>18</v>
@@ -2274,7 +2284,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>28</v>
@@ -2282,36 +2292,36 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2322,13 +2332,13 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>28</v>
@@ -2340,20 +2350,20 @@
         <v>33</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>30</v>
@@ -2361,24 +2371,24 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>36</v>
@@ -2391,13 +2401,13 @@
         <v>24</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>39</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>31</v>
@@ -2410,22 +2420,22 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>19</v>
@@ -2450,34 +2460,32 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>169</v>
+        <v>284</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2487,16 +2495,16 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>84</v>
@@ -2505,18 +2513,18 @@
         <v>27</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -2526,13 +2534,13 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>28</v>
@@ -2541,10 +2549,10 @@
         <v>39</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -2552,10 +2560,10 @@
         <v>28</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2566,16 +2574,16 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>14</v>
@@ -2605,16 +2613,16 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -2624,7 +2632,7 @@
         <v>28</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>54</v>
@@ -2633,10 +2641,10 @@
         <v>38</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2646,13 +2654,13 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>81</v>
@@ -2675,7 +2683,7 @@
         <v>29</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -2685,13 +2693,13 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>40</v>
@@ -2716,10 +2724,10 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>89</v>
@@ -2740,7 +2748,7 @@
         <v>67</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>81</v>
@@ -2749,12 +2757,12 @@
         <v>45</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="P30" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -2762,35 +2770,35 @@
         <v>9</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2801,22 +2809,22 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>28</v>
@@ -2831,10 +2839,10 @@
         <v>28</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>39</v>
+        <v>280</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -2844,10 +2852,10 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>48</v>
@@ -2859,7 +2867,7 @@
         <v>29</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>28</v>
@@ -2877,10 +2885,10 @@
         <v>79</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="N33" s="2"/>
       <c r="P33" s="2" t="s">
@@ -2889,13 +2897,13 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>28</v>
@@ -2907,7 +2915,7 @@
         <v>22</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2" t="s">
@@ -2917,26 +2925,26 @@
         <v>38</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="M34" s="4"/>
       <c r="N34" s="2"/>
       <c r="P34" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>28</v>
@@ -2954,7 +2962,7 @@
         <v>84</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>81</v>
@@ -2963,10 +2971,10 @@
         <v>79</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="N35" s="2"/>
       <c r="P35" s="2" t="s">
@@ -2975,16 +2983,16 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>14</v>
@@ -2993,7 +3001,7 @@
         <v>22</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2" t="s">
@@ -3003,10 +3011,10 @@
         <v>58</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="2"/>
@@ -3016,10 +3024,10 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>52</v>
@@ -3040,19 +3048,19 @@
         <v>84</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>29</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="N37" s="2"/>
       <c r="P37" s="2" t="s">
@@ -3061,13 +3069,13 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>38</v>
@@ -3082,7 +3090,7 @@
         <v>28</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>33</v>
@@ -3091,10 +3099,10 @@
         <v>81</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="M38" s="4"/>
       <c r="N38" s="2"/>
@@ -3104,29 +3112,29 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>81</v>
@@ -3135,10 +3143,10 @@
         <v>29</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="N39" s="2"/>
       <c r="P39" s="2" t="s">
@@ -3147,22 +3155,22 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>28</v>
@@ -3177,26 +3185,26 @@
         <v>38</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="M40" s="4"/>
       <c r="N40" s="2"/>
       <c r="P40" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>28</v>
@@ -3211,19 +3219,19 @@
         <v>81</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>54</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -3233,13 +3241,13 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>81</v>
@@ -3257,7 +3265,7 @@
         <v>84</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>40</v>
@@ -3268,7 +3276,7 @@
         <v>31</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="P42" s="2" t="s">
         <v>62</v>
@@ -3276,28 +3284,28 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>25</v>
@@ -3308,30 +3316,30 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>36</v>
@@ -3343,10 +3351,10 @@
         <v>29</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
@@ -3362,10 +3370,10 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>52</v>
@@ -3377,13 +3385,13 @@
         <v>39</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>27</v>
@@ -3392,10 +3400,10 @@
         <v>81</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>

</xml_diff>

<commit_message>
fix some errors in signals.xlsx and ID.vhd can compile sucessfully but I'm not sure that it is right
</commit_message>
<xml_diff>
--- a/datapath/信号表.xlsx
+++ b/datapath/信号表.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="287">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1173,6 +1173,10 @@
   </si>
   <si>
     <t>PC+1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1521,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2085,9 @@
       <c r="F13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>286</v>
+      </c>
       <c r="H13" s="2" t="s">
         <v>84</v>
       </c>
@@ -3044,9 +3050,7 @@
       <c r="G37" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="H37" s="2"/>
       <c r="I37" s="2" t="s">
         <v>226</v>
       </c>

</xml_diff>